<commit_message>
Add report template and fix bug
</commit_message>
<xml_diff>
--- a/HotelManagement/Assets/XLSXTemplate/Invoice_template.xlsx
+++ b/HotelManagement/Assets/XLSXTemplate/Invoice_template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE75C57-1DED-4F89-8CC8-F44AB9E56D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A7DD00-892D-4A3B-B2E6-3C0358AC0EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30810" yWindow="2130" windowWidth="25890" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Service Invoice" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>QUANTITY</t>
   </si>
@@ -216,9 +216,6 @@
     <t>KTX Khu B, ĐHQG TP HCM</t>
   </si>
   <si>
-    <t>5/7/2021</t>
-  </si>
-  <si>
     <t>7/7/2021</t>
   </si>
 </sst>
@@ -226,11 +223,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="_([$VND]\ * #,##0_);_([$VND]\ * \(#,##0\);_([$VND]\ * &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="[$VND]\ #,##0"/>
+    <numFmt numFmtId="166" formatCode="[$VND]\ #,##0"/>
+    <numFmt numFmtId="168" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
   <fonts count="38" x14ac:knownFonts="1">
     <font>
@@ -628,7 +626,7 @@
     </xf>
     <xf numFmtId="44" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -821,16 +819,16 @@
     <xf numFmtId="2" fontId="31" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="31" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="31" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="31" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="31" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="31" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="31" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="165" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -848,17 +846,20 @@
     <xf numFmtId="165" fontId="31" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -1307,7 +1308,7 @@
   <dimension ref="B1:J34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1333,13 +1334,13 @@
       </c>
       <c r="D1" s="41"/>
       <c r="E1" s="42"/>
-      <c r="F1" s="85" t="s">
+      <c r="F1" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
     </row>
     <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="32"/>
@@ -1386,15 +1387,15 @@
         <v>23</v>
       </c>
       <c r="D5" s="36"/>
-      <c r="E5" s="56">
+      <c r="E5" s="86">
         <v>123456789</v>
       </c>
       <c r="G5" s="36"/>
       <c r="H5" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="88" t="s">
-        <v>29</v>
+      <c r="I5" s="85" t="s">
+        <v>28</v>
       </c>
       <c r="J5" s="36"/>
     </row>
@@ -1417,8 +1418,8 @@
         <v>25</v>
       </c>
       <c r="D7" s="36"/>
-      <c r="E7" s="86" t="s">
-        <v>28</v>
+      <c r="E7" s="88">
+        <v>44382</v>
       </c>
       <c r="G7" s="30"/>
       <c r="H7" s="30"/>
@@ -1430,8 +1431,8 @@
         <v>26</v>
       </c>
       <c r="D8" s="36"/>
-      <c r="E8" s="87" t="s">
-        <v>28</v>
+      <c r="E8" s="89">
+        <v>44384</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
@@ -1497,7 +1498,7 @@
       </c>
       <c r="F12" s="74">
         <f>IF(DATEDIF(E7,E8,"d")=0, 1, DATEDIF(E7,E8,"d"))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" s="75">
         <v>1.5</v>
@@ -1507,7 +1508,7 @@
       </c>
       <c r="I12" s="83">
         <f>F12*G12*H12</f>
-        <v>375000</v>
+        <v>750000</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1638,7 +1639,7 @@
       </c>
       <c r="I22" s="70">
         <f>SUM(I12:I20)</f>
-        <v>375000</v>
+        <v>750000</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1655,7 +1656,7 @@
       </c>
       <c r="I23" s="80">
         <f>I22*H23</f>
-        <v>93750</v>
+        <v>187500</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1670,7 +1671,7 @@
       </c>
       <c r="I24" s="73">
         <f>IF(SUM(I22)&gt;0,SUM(I22,I23),"")</f>
-        <v>468750</v>
+        <v>937500</v>
       </c>
     </row>
     <row r="26" spans="2:9" s="26" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update template and fix minor ui
</commit_message>
<xml_diff>
--- a/HotelManagement/Assets/XLSXTemplate/Invoice_template.xlsx
+++ b/HotelManagement/Assets/XLSXTemplate/Invoice_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A7DD00-892D-4A3B-B2E6-3C0358AC0EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC1B8D9-9DA0-4DD9-9F17-A76277009825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -213,10 +213,10 @@
     <t>Ngày trả phòng:</t>
   </si>
   <si>
-    <t>KTX Khu B, ĐHQG TP HCM</t>
-  </si>
-  <si>
     <t>7/7/2021</t>
+  </si>
+  <si>
+    <t>TP Hồ Chí Minh</t>
   </si>
 </sst>
 </file>
@@ -228,7 +228,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="_([$VND]\ * #,##0_);_([$VND]\ * \(#,##0\);_([$VND]\ * &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="[$VND]\ #,##0"/>
-    <numFmt numFmtId="168" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
   <fonts count="38" x14ac:knownFonts="1">
     <font>
@@ -626,7 +626,7 @@
     </xf>
     <xf numFmtId="44" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -689,9 +689,6 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="6">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="7">
       <alignment horizontal="center" vertical="center"/>
@@ -763,7 +760,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="31" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -852,14 +848,23 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="167" fontId="19" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -1308,7 +1313,7 @@
   <dimension ref="B1:J34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1328,110 +1333,111 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="32"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="87" t="s">
+      <c r="D1" s="40"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
     </row>
     <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="32"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
     </row>
     <row r="3" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="33"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
     </row>
     <row r="4" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="36" t="s">
+      <c r="D4" s="28"/>
+      <c r="E4" s="35" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="81" t="s">
+      <c r="H4" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="82">
+      <c r="I4" s="80">
         <v>1</v>
       </c>
       <c r="J4" s="13"/>
     </row>
     <row r="5" spans="2:10" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="86">
+      <c r="D5" s="35"/>
+      <c r="E5" s="84">
         <v>123456789</v>
       </c>
-      <c r="G5" s="36"/>
-      <c r="H5" s="81" t="s">
+      <c r="G5" s="35"/>
+      <c r="H5" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="85" t="s">
+      <c r="I5" s="83" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="35"/>
+    </row>
+    <row r="6" spans="2:10" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="7"/>
+      <c r="C6" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="35"/>
+      <c r="E6" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="36"/>
-    </row>
-    <row r="6" spans="2:10" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
-      <c r="C6" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="25"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
       <c r="H6" s="24"/>
-      <c r="I6" s="30"/>
+      <c r="I6" s="29"/>
     </row>
     <row r="7" spans="2:10" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="88">
+      <c r="D7" s="35"/>
+      <c r="E7" s="85">
         <v>44382</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
       <c r="I7" s="11"/>
     </row>
     <row r="8" spans="2:10" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="89">
+      <c r="D8" s="35"/>
+      <c r="E8" s="86">
         <v>44384</v>
       </c>
       <c r="F8" s="18"/>
@@ -1440,21 +1446,21 @@
       <c r="I8" s="12"/>
     </row>
     <row r="9" spans="2:10" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
     </row>
     <row r="10" spans="2:10" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
-      <c r="F10" s="40"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="10"/>
@@ -1463,276 +1469,277 @@
       <c r="B11" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="51" t="s">
+      <c r="E11" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="51" t="s">
+      <c r="F11" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="50" t="s">
+      <c r="G11" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="50" t="s">
+      <c r="H11" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="52" t="s">
+      <c r="I11" s="51" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="15"/>
-      <c r="C12" s="57">
+      <c r="C12" s="55">
         <v>1</v>
       </c>
-      <c r="D12" s="58">
+      <c r="D12" s="56">
         <v>911</v>
       </c>
-      <c r="E12" s="59">
+      <c r="E12" s="57">
         <v>3</v>
       </c>
-      <c r="F12" s="74">
+      <c r="F12" s="72">
         <f>IF(DATEDIF(E7,E8,"d")=0, 1, DATEDIF(E7,E8,"d"))</f>
         <v>2</v>
       </c>
-      <c r="G12" s="75">
+      <c r="G12" s="73">
         <v>1.5</v>
       </c>
-      <c r="H12" s="84">
+      <c r="H12" s="82">
         <v>250000</v>
       </c>
-      <c r="I12" s="83">
+      <c r="I12" s="81">
         <f>F12*G12*H12</f>
         <v>750000</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="15"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="77"/>
-      <c r="I13" s="78"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="76"/>
     </row>
     <row r="14" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="15"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="76"/>
-      <c r="I14" s="79" t="str">
+      <c r="C14" s="55"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="77" t="str">
         <f t="shared" ref="I14:I21" si="0">IF(SUM(C14)&gt;0,SUM(C14*F14),"")</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="15"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="63" t="s">
+      <c r="C15" s="60"/>
+      <c r="D15" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="64"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="78" t="str">
+      <c r="E15" s="62"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="75"/>
+      <c r="I15" s="76" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="16" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="15"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="76"/>
-      <c r="I16" s="79" t="str">
+      <c r="C16" s="55"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="74"/>
+      <c r="I16" s="77" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="17" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="15"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="77"/>
-      <c r="I17" s="78" t="str">
+      <c r="C17" s="60"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="75"/>
+      <c r="I17" s="76" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="18" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="15"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="76"/>
-      <c r="I18" s="79" t="str">
+      <c r="C18" s="55"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="74"/>
+      <c r="I18" s="77" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="19" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="15"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="66"/>
-      <c r="H19" s="77"/>
-      <c r="I19" s="78" t="str">
+      <c r="C19" s="60"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="64"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="76" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="20" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="15"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="76"/>
-      <c r="I20" s="79" t="str">
+      <c r="C20" s="55"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="77" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="21" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="15"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="66"/>
-      <c r="I21" s="67" t="str">
+      <c r="C21" s="60"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="65" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="22" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="16"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="69"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="44" t="s">
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="70">
+      <c r="I22" s="68">
         <f>SUM(I12:I20)</f>
         <v>750000</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="17"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="45" t="s">
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="H23" s="46">
+      <c r="H23" s="45">
         <v>0.25</v>
       </c>
-      <c r="I23" s="80">
+      <c r="I23" s="78">
         <f>I22*H23</f>
         <v>187500</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="17"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="72" t="s">
+      <c r="C24" s="66"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="I24" s="73">
+      <c r="I24" s="71">
         <f>IF(SUM(I22)&gt;0,SUM(I22,I23),"")</f>
         <v>937500</v>
       </c>
     </row>
-    <row r="26" spans="2:9" s="26" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
+    <row r="26" spans="2:9" s="25" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
     </row>
     <row r="27" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C27" s="38"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
     </row>
     <row r="28" spans="2:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C28" s="3"/>
-      <c r="D28" s="48" t="s">
+      <c r="D28" s="47" t="s">
         <v>15</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="19"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="48" t="s">
+      <c r="H28" s="47" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="29" spans="2:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D29" s="53" t="s">
+      <c r="D29" s="52" t="s">
         <v>13</v>
       </c>
       <c r="G29" s="2"/>
-      <c r="H29" s="53" t="s">
+      <c r="H29" s="52" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="6"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
       <c r="F30" s="21"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
-      <c r="I30" s="31"/>
+      <c r="I30" s="30"/>
     </row>
     <row r="33" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H34" s="48" t="s">
+      <c r="H34" s="47" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="F1:J1"/>
+    <mergeCell ref="E6:G6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -1762,12 +1769,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="2:2" ht="162" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>